<commit_message>
addscrapy and process and thread
</commit_message>
<xml_diff>
--- a/python/Spider/Top250.xlsx
+++ b/python/Spider/Top250.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="550" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -197,7 +197,7 @@
     <t> / 飘</t>
   </si>
   <si>
-    <t>导演: 维克多·弗莱明 Victor Fleming / 乔治·库克 George Cukor   主演: 克/1940 / 美国 / 剧情 爱情 战争</t>
+    <t>导演: 维克多·弗莱明 Victor Fleming / 乔治·库克 George Cukor   主演: 托/1939 / 美国 / 剧情 历史 爱情 战争</t>
   </si>
   <si>
     <t>天堂电影院 / Nuovo Cinema Paradiso</t>
@@ -281,6 +281,24 @@
     <t>导演: 彼得·杰克逊 Peter Jackson   主演: 维果·莫腾森 Viggo Mortensen / /2003 / 美国 新西兰 / 剧情 动作 奇幻 冒险</t>
   </si>
   <si>
+    <t>星际穿越 / Interstellar</t>
+  </si>
+  <si>
+    <t> / 星际启示录(港)  /  星际效应(台)</t>
+  </si>
+  <si>
+    <t>导演: 克里斯托弗·诺兰 Christopher Nolan   主演: 马修·麦康纳 Matthew Mc/2014 / 美国 英国 加拿大 / 剧情 科幻 冒险</t>
+  </si>
+  <si>
+    <t>少年派的奇幻漂流 / Life of Pi</t>
+  </si>
+  <si>
+    <t> / 少年Pi的奇幻漂流  /  漂流少年Pi</t>
+  </si>
+  <si>
+    <t>导演: 李安 Ang Lee   主演: 苏拉·沙玛 Suraj Sharma / 拉菲·斯波 Rafe Spa/2012 / 美国 台湾 英国 加拿大 / 剧情 奇幻 冒险</t>
+  </si>
+  <si>
     <t>天空之城 / 天空の城ラピュタ</t>
   </si>
   <si>
@@ -290,24 +308,6 @@
     <t>导演: 宫崎骏 Hayao Miyazaki   主演: 田中真弓 Mayumi Tanaka / 横泽启子 Ke/1986 / 日本 / 动画 奇幻 冒险</t>
   </si>
   <si>
-    <t>少年派的奇幻漂流 / Life of Pi</t>
-  </si>
-  <si>
-    <t> / 少年Pi的奇幻漂流  /  漂流少年Pi</t>
-  </si>
-  <si>
-    <t>导演: 李安 Ang Lee   主演: 苏拉·沙玛 Suraj Sharma / 拉菲·斯波 Rafe Spa/2012 / 美国 台湾 英国 加拿大 / 剧情 奇幻 冒险</t>
-  </si>
-  <si>
-    <t>星际穿越 / Interstellar</t>
-  </si>
-  <si>
-    <t> / 星际启示录(港)  /  星际效应(台)</t>
-  </si>
-  <si>
-    <t>导演: 克里斯托弗·诺兰 Christopher Nolan   主演: 马修·麦康纳 Matthew Mc/2014 / 美国 英国 加拿大 / 剧情 科幻 冒险</t>
-  </si>
-  <si>
     <t>罗马假日 / Roman Holiday</t>
   </si>
   <si>
@@ -488,6 +488,15 @@
     <t>导演: 让-皮埃尔·热内 Jean-Pierre Jeunet   主演: 奥黛丽·塔图 Audrey Tau/2001 / 法国 德国 / 喜剧 爱情</t>
   </si>
   <si>
+    <t>控方证人 / Witness for the Prosecution</t>
+  </si>
+  <si>
+    <t> / 雄才伟略  /  情妇</t>
+  </si>
+  <si>
+    <t>导演: 比利·怀尔德 Billy Wilder   主演: 查尔斯·劳顿 Charles Laughton / /1957 / 美国 / 剧情 犯罪 悬疑</t>
+  </si>
+  <si>
     <t>美国往事 / Once Upon a Time in America</t>
   </si>
   <si>
@@ -497,13 +506,13 @@
     <t>导演: 赛尔乔·莱翁内 Sergio Leone   主演: 罗伯特·德尼罗 Robert De Niro /1984 / 意大利 美国 / 犯罪 剧情</t>
   </si>
   <si>
-    <t>控方证人 / Witness for the Prosecution</t>
-  </si>
-  <si>
-    <t> / 雄才伟略  /  情妇</t>
-  </si>
-  <si>
-    <t>导演: 比利·怀尔德 Billy Wilder   主演: 查尔斯·劳顿 Charles Laughton / /1957 / 美国 / 剧情 犯罪 悬疑</t>
+    <t>钢琴家 / The Pianist</t>
+  </si>
+  <si>
+    <t> / 战地琴人  /  钢琴战曲</t>
+  </si>
+  <si>
+    <t>导演: 罗曼·波兰斯基 Roman Polanski   主演: 艾德里安·布洛迪 Adrien Brod/2002 / 法国 德国 英国 波兰 / 剧情 传记 历史 战争</t>
   </si>
   <si>
     <t>七宗罪 / Se7en</t>
@@ -515,13 +524,13 @@
     <t>导演: 大卫·芬奇 David Fincher   主演: 摩根·弗里曼 Morgan Freeman / 布/1995 / 美国 / 剧情 犯罪 悬疑 惊悚</t>
   </si>
   <si>
-    <t>钢琴家 / The Pianist</t>
-  </si>
-  <si>
-    <t> / 战地琴人  /  钢琴战曲</t>
-  </si>
-  <si>
-    <t>导演: 罗曼·波兰斯基 Roman Polanski   主演: 艾德里安·布洛迪 Adrien Brod/2002 / 法国 德国 英国 波兰 / 剧情 传记 历史 战争</t>
+    <t>辩护人 / 변호인</t>
+  </si>
+  <si>
+    <t> / 逆权大状(港)  /  正义辩护人(台)</t>
+  </si>
+  <si>
+    <t>导演: 杨宇硕 Woo-seok Yang   主演: 宋康昊 Kang-ho Song / 吴达洙 Dal-su O/2013 / 韩国 / 剧情</t>
   </si>
   <si>
     <t>狮子王 / The Lion King</t>
@@ -531,15 +540,6 @@
   </si>
   <si>
     <t>导演: Roger Allers / 罗伯·明可夫 Rob Minkoff   主演: 乔纳森·泰勒·托马/1994 / 美国 / 剧情 动画 冒险 歌舞 家庭</t>
-  </si>
-  <si>
-    <t>辩护人 / 변호인</t>
-  </si>
-  <si>
-    <t> / 逆权大状(港)  /  正义辩护人(台)</t>
-  </si>
-  <si>
-    <t>导演: 杨宇硕 Woo-seok Yang   主演: 宋康昊 Kang-ho Song / 吴达洙 Dal-su O/2013 / 韩国 / 剧情</t>
   </si>
   <si>
     <t>饮食男女 / 飲食男女</t>
@@ -670,6 +670,15 @@
     <t>导演: 李濬益 Jun-ik Lee   主演: 薛景求 Kyung-gu Sol / 严志媛 Ji-won Uhm /2013 / 韩国 / 剧情 家庭</t>
   </si>
   <si>
+    <t>拯救大兵瑞恩 / Saving Private Ryan</t>
+  </si>
+  <si>
+    <t> / 雷霆救兵(港)  /  抢救雷恩大兵(台)</t>
+  </si>
+  <si>
+    <t>导演: 史蒂文·斯皮尔伯格 Steven Spielberg   主演: 汤姆·汉克斯 Tom Hanks/1998 / 美国 / 剧情 历史 战争</t>
+  </si>
+  <si>
     <t>蝴蝶效应 / The Butterfly Effect</t>
   </si>
   <si>
@@ -679,13 +688,13 @@
     <t>导演: 埃里克·布雷斯 Eric Bress / J·麦基·格鲁伯 J. Mackye Gruber   主/2004 / 美国 加拿大 / 剧情 悬疑 科幻 惊悚</t>
   </si>
   <si>
-    <t>拯救大兵瑞恩 / Saving Private Ryan</t>
-  </si>
-  <si>
-    <t> / 雷霆救兵(港)  /  抢救雷恩大兵(台)</t>
-  </si>
-  <si>
-    <t>导演: 史蒂文·斯皮尔伯格 Steven Spielberg   主演: 汤姆·汉克斯 Tom Hanks/1998 / 美国 / 剧情 历史 战争</t>
+    <t>疯狂动物城 / Zootopia</t>
+  </si>
+  <si>
+    <t> / 优兽大都会(港)  /  动物方城市(台)</t>
+  </si>
+  <si>
+    <t>导演: 拜伦·霍华德 Byron Howard / 瑞奇·摩尔 Rich Moore   主演: 金妮弗·/2016 / 美国 / 喜剧 动画 冒险</t>
   </si>
   <si>
     <t>西西里的美丽传说 / Malèna</t>
@@ -706,15 +715,6 @@
     <t>导演: Adam Elliot   主演: 托妮·科莱特 Toni Collette / 菲利普·塞默·霍/2009 / 澳大利亚 / 剧情 爱情 动画</t>
   </si>
   <si>
-    <t>疯狂动物城 / Zootopia</t>
-  </si>
-  <si>
-    <t> / 优兽大都会(港)  /  动物方城市(台)</t>
-  </si>
-  <si>
-    <t>导演: 拜伦·霍华德 Byron Howard / 瑞奇·摩尔 Rich Moore   主演: 金妮弗·/2016 / 美国 / 喜剧 动画 冒险</t>
-  </si>
-  <si>
     <t>心灵捕手 / Good Will Hunting</t>
   </si>
   <si>
@@ -724,6 +724,15 @@
     <t>导演: 格斯·范·桑特 Gus Van Sant   主演: 马特·达蒙 Matt Damon / 罗宾·/1997 / 美国 / 剧情</t>
   </si>
   <si>
+    <t>春光乍泄 / 春光乍洩</t>
+  </si>
+  <si>
+    <t> / 一起快乐  /  Happy Together</t>
+  </si>
+  <si>
+    <t>导演: 王家卫 Kar Wai Wong   主演: 张国荣 Leslie Cheung / 梁朝伟 Tony Leu/1997 / 香港 日本 韩国 / 剧情 爱情 同性</t>
+  </si>
+  <si>
     <t>幽灵公主 / もののけ姫</t>
   </si>
   <si>
@@ -733,13 +742,13 @@
     <t>导演: 宫崎骏 Hayao Miyazaki   主演: 松田洋治 Yôji Matsuda / 石田百合/1997 / 日本 / 动作 爱情 战争 动画 奇幻 冒险</t>
   </si>
   <si>
-    <t>春光乍泄 / 春光乍洩</t>
-  </si>
-  <si>
-    <t> / 一起快乐  /  Happy Together</t>
-  </si>
-  <si>
-    <t>导演: 王家卫 Kar Wai Wong   主演: 张国荣 Leslie Cheung / 梁朝伟 Tony Leu/1997 / 香港 日本 韩国 / 剧情 爱情 同性</t>
+    <t>让子弹飞</t>
+  </si>
+  <si>
+    <t> / 让子弹飞一会儿  /  火烧云</t>
+  </si>
+  <si>
+    <t>导演: 姜文 Wen Jiang   主演: 姜文 Wen Jiang / 葛优 You Ge / 周润发 Yun-F/2010 / 中国大陆 香港 / 剧情 喜剧 动作 西部</t>
   </si>
   <si>
     <t>第六感 / The Sixth Sense</t>
@@ -760,15 +769,6 @@
     <t>导演: 姜文 Wen Jiang   主演: 夏雨 Yu Xia / 宁静 Jing Ning / 陶虹 Hong Tao1994 / 中国大陆 香港 / 剧情</t>
   </si>
   <si>
-    <t>让子弹飞</t>
-  </si>
-  <si>
-    <t> / 让子弹飞一会儿  /  火烧云</t>
-  </si>
-  <si>
-    <t>导演: 姜文 Wen Jiang   主演: 姜文 Wen Jiang / 葛优 You Ge / 周润发 Yun-F/2010 / 中国大陆 香港 / 剧情 喜剧 动作 西部</t>
-  </si>
-  <si>
     <t>大闹天宫</t>
   </si>
   <si>
@@ -814,6 +814,24 @@
     <t>导演: Kátia Lund / Fernando Meirelles   主演: Alexandre Rodrigues / Lea/2002 / 巴西 法国 / 犯罪 剧情</t>
   </si>
   <si>
+    <t>禁闭岛 / Shutter Island</t>
+  </si>
+  <si>
+    <t> / 不赦岛(港)  /  隔离岛(台)</t>
+  </si>
+  <si>
+    <t>导演: Martin Scorsese   主演: 莱昂纳多·迪卡普里奥 Leonardo DiCaprio / /2010 / 美国 / 剧情 悬疑 惊悚</t>
+  </si>
+  <si>
+    <t>甜蜜蜜</t>
+  </si>
+  <si>
+    <t> / Comrades: Almost a Love Story</t>
+  </si>
+  <si>
+    <t>导演: 陈可辛 Peter Chan   主演: 黎明 Leon Lai / 张曼玉 Maggie Cheung / /1996 / 香港 / 剧情 爱情</t>
+  </si>
+  <si>
     <t>阳光姐妹淘 / 써니</t>
   </si>
   <si>
@@ -823,24 +841,6 @@
     <t>导演: 姜炯哲 Hyeong-Cheol Kang   主演: 沈恩京 Eun-kyung Shim / 闵孝琳 Hy/2011 / 韩国 / 剧情 喜剧</t>
   </si>
   <si>
-    <t>甜蜜蜜</t>
-  </si>
-  <si>
-    <t> / Comrades: Almost a Love Story</t>
-  </si>
-  <si>
-    <t>导演: 陈可辛 Peter Chan   主演: 黎明 Leon Lai / 张曼玉 Maggie Cheung / /1996 / 香港 / 剧情 爱情</t>
-  </si>
-  <si>
-    <t>禁闭岛 / Shutter Island</t>
-  </si>
-  <si>
-    <t> / 不赦岛(港)  /  隔离岛(台)</t>
-  </si>
-  <si>
-    <t>导演: Martin Scorsese   主演: 莱昂纳多·迪卡普里奥 Leonardo DiCaprio / /2010 / 美国 / 剧情 悬疑 惊悚</t>
-  </si>
-  <si>
     <t>致命ID / Identity</t>
   </si>
   <si>
@@ -1003,6 +1003,15 @@
     <t>导演: 迪恩·德布洛斯 Dean DeBlois / 克里斯·桑德斯 Chris Sanders   主演:/2010 / 美国 / 喜剧 动画 奇幻 冒险 家庭</t>
   </si>
   <si>
+    <t>穿条纹睡衣的男孩 / The Boy in the Striped Pajamas</t>
+  </si>
+  <si>
+    <t> / 穿条纹衣服的男孩  /  穿条纹衣的男孩</t>
+  </si>
+  <si>
+    <t>导演: 马克·赫门 Mark Herman   主演: 阿沙·巴特菲尔德 Asa Butterfield / /2008 / 英国 美国 / 剧情 战争</t>
+  </si>
+  <si>
     <t>超脱 / Detachment</t>
   </si>
   <si>
@@ -1012,13 +1021,13 @@
     <t>导演: 托尼·凯耶 Tony Kaye   主演: 艾德里安·布洛迪 Adrien Brody / 克里/2011 / 美国 / 剧情</t>
   </si>
   <si>
-    <t>穿条纹睡衣的男孩 / The Boy in the Striped Pajamas</t>
-  </si>
-  <si>
-    <t> / 穿条纹衣服的男孩  /  穿条纹衣的男孩</t>
-  </si>
-  <si>
-    <t>导演: 马克·赫门 Mark Herman   主演: 阿沙·巴特菲尔德 Asa Butterfield / /2008 / 英国 美国 / 剧情 战争</t>
+    <t>消失的爱人 / Gone Girl</t>
+  </si>
+  <si>
+    <t> / 失踪的女孩  /  失踪女孩</t>
+  </si>
+  <si>
+    <t>导演: 大卫·芬奇 David Fincher   主演: 本·阿弗莱克 Ben Affleck / 罗莎蒙/2014 / 美国 / 剧情 犯罪 悬疑 惊悚</t>
   </si>
   <si>
     <t>海洋 / Océans</t>
@@ -1039,15 +1048,6 @@
     <t>导演: 史蒂文·斯皮尔伯格 Steven Spielberg   主演: 汤姆·汉克斯 Tom Hanks/2004 / 美国 / 喜剧 剧情 爱情</t>
   </si>
   <si>
-    <t>消失的爱人 / Gone Girl</t>
-  </si>
-  <si>
-    <t> / 失踪的女孩  /  失踪女孩</t>
-  </si>
-  <si>
-    <t>导演: 大卫·芬奇 David Fincher   主演: 本·阿弗莱克 Ben Affleck / 罗莎蒙/2014 / 美国 / 剧情 犯罪 悬疑 惊悚</t>
-  </si>
-  <si>
     <t>菊次郎的夏天 / 菊次郎の夏</t>
   </si>
   <si>
@@ -1084,6 +1084,24 @@
     <t>导演: 黑泽明 Akira Kurosawa   主演: 三船敏郎 Toshirô Mifune / 志村乔 /1954 / 日本 / 动作 冒险 剧情</t>
   </si>
   <si>
+    <t>恐怖直播 / 더 테러 라이브</t>
+  </si>
+  <si>
+    <t> / 死亡“动”新闻(港)  /  恐怖攻击直播(台)</t>
+  </si>
+  <si>
+    <t>导演: 金秉祐 Byeong-woo Kim   主演: 河正宇 Jung-woo Ha / 李璟荣 Kyeong-y/2013 / 韩国 / 剧情 犯罪 悬疑</t>
+  </si>
+  <si>
+    <t>岁月神偷 / 歲月神偷</t>
+  </si>
+  <si>
+    <t> / 1969太空漫游  /  Echoes Of The Rainbow</t>
+  </si>
+  <si>
+    <t>导演: 罗启锐 Alex Law   主演: 吴君如 Sandra Ng / 任达华 Simon Yam / 钟绍/2010 / 香港 中国大陆 / 剧情 家庭</t>
+  </si>
+  <si>
     <t>电锯惊魂 / Saw</t>
   </si>
   <si>
@@ -1093,15 +1111,6 @@
     <t>导演: 詹姆斯·温 James Wan   主演: 雷·沃纳尔 Leigh Whannell / 加利·艾/2004 / 美国 澳大利亚 / 犯罪 悬疑 惊悚</t>
   </si>
   <si>
-    <t>岁月神偷 / 歲月神偷</t>
-  </si>
-  <si>
-    <t> / 1969太空漫游  /  Echoes Of The Rainbow</t>
-  </si>
-  <si>
-    <t>导演: 罗启锐 Alex Law   主演: 吴君如 Sandra Ng / 任达华 Simon Yam / 钟绍/2010 / 香港 中国大陆 / 剧情 家庭</t>
-  </si>
-  <si>
     <t>谍影重重3 / The Bourne Ultimatum</t>
   </si>
   <si>
@@ -1111,13 +1120,13 @@
     <t>导演: 保罗·格林格拉斯 Paul Greengrass   主演: 马特·达蒙 Matt Damon / /2007 / 美国 德国 / 动作 悬疑 惊悚</t>
   </si>
   <si>
-    <t>恐怖直播 / 더 테러 라이브</t>
-  </si>
-  <si>
-    <t> / 死亡“动”新闻(港)  /  恐怖攻击直播(台)</t>
-  </si>
-  <si>
-    <t>导演: 金秉祐 Byeong-woo Kim   主演: 河正宇 Jung-woo Ha / 李璟荣 Kyeong-y/2013 / 韩国 / 剧情 犯罪 悬疑</t>
+    <t>借东西的小人阿莉埃蒂 / 借りぐらしのアリエッティ</t>
+  </si>
+  <si>
+    <t> / 借物少女艾莉缇(台)  /  借东西的小矮人亚莉亚蒂(港)</t>
+  </si>
+  <si>
+    <t>导演: 米林宏昌 Hiromasa Yonebayashi   主演: 志田未来 Mirai Shida / 神木/2010 / 日本 / 动画 奇幻 冒险</t>
   </si>
   <si>
     <t>燃情岁月 / Legends of the Fall</t>
@@ -1129,15 +1138,6 @@
     <t>导演: 爱德华·兹威克 Edward Zwick   主演: 安东尼·霍普金斯 Anthony Hopki/1994 / 美国 / 剧情 爱情 西部 家庭</t>
   </si>
   <si>
-    <t>借东西的小人阿莉埃蒂 / 借りぐらしのアリエッティ</t>
-  </si>
-  <si>
-    <t> / 借物少女艾莉缇(台)  /  借东西的小矮人亚莉亚蒂(港)</t>
-  </si>
-  <si>
-    <t>导演: 米林宏昌 Hiromasa Yonebayashi   主演: 志田未来 Mirai Shida / 神木/2010 / 日本 / 动画 奇幻 冒险</t>
-  </si>
-  <si>
     <t>真爱至上 / Love Actually</t>
   </si>
   <si>
@@ -1156,6 +1156,15 @@
     <t>导演: 巴瑞·莱文森 Barry Levinson   主演: 达斯汀·霍夫曼 Dustin Hoffman /1988 / 美国 / 剧情</t>
   </si>
   <si>
+    <t>红辣椒 / パプリカ</t>
+  </si>
+  <si>
+    <t> / 盗梦侦探  /  帕布莉卡</t>
+  </si>
+  <si>
+    <t>导演: 今敏 Satoshi Kon   主演: 林原惠美 Megumi Hayashibara / 古谷彻 T/2006 / 日本 / 动画 悬疑 科幻 惊悚</t>
+  </si>
+  <si>
     <t>贫民窟的百万富翁 / Slumdog Millionaire</t>
   </si>
   <si>
@@ -1165,13 +1174,22 @@
     <t>导演: 丹尼·鲍尔 Danny Boyle / 洛芙琳·坦丹 Loveleen Tandan   主演: 戴夫/2008 / 英国 美国 / 剧情 爱情</t>
   </si>
   <si>
-    <t>红辣椒 / パプリカ</t>
-  </si>
-  <si>
-    <t> / 盗梦侦探  /  帕布莉卡</t>
-  </si>
-  <si>
-    <t>导演: 今敏 Satoshi Kon   主演: 林原惠美 Megumi Hayashibara / 古谷彻 T/2006 / 日本 / 动画 悬疑 科幻 惊悚</t>
+    <t>杀人回忆 / 살인의 추억</t>
+  </si>
+  <si>
+    <t> / 谋杀回忆  /  杀手回忆录</t>
+  </si>
+  <si>
+    <t>导演: 奉俊昊 Joon-ho Bong   主演: 宋康昊 Kang-ho Song / 金相庆 Sang-kyun/2003 / 韩国 / 犯罪 剧情 悬疑 惊悚</t>
+  </si>
+  <si>
+    <t>东邪西毒 / 東邪西毒</t>
+  </si>
+  <si>
+    <t> / Ashes of Time</t>
+  </si>
+  <si>
+    <t>导演: 王家卫 Kar Wai Wong   主演: 张国荣 Leslie Cheung / 张曼玉 Maggie C/1994 / 香港 台湾 / 剧情 动作 爱情 武侠 古装</t>
   </si>
   <si>
     <t>虎口脱险 / La grande vadrouille</t>
@@ -1183,24 +1201,6 @@
     <t>导演: 杰拉尔·乌里 Gérard Oury   主演: 路易·德·菲耐斯 Louis de Funès/1966 / 法国 英国 / 喜剧 战争</t>
   </si>
   <si>
-    <t>东邪西毒 / 東邪西毒</t>
-  </si>
-  <si>
-    <t> / Ashes of Time</t>
-  </si>
-  <si>
-    <t>导演: 王家卫 Kar Wai Wong   主演: 张国荣 Leslie Cheung / 张曼玉 Maggie C/1994 / 香港 台湾 / 剧情 动作 爱情 武侠 古装</t>
-  </si>
-  <si>
-    <t>杀人回忆 / 살인의 추억</t>
-  </si>
-  <si>
-    <t> / 谋杀回忆  /  杀手回忆录</t>
-  </si>
-  <si>
-    <t>导演: 奉俊昊 Joon-ho Bong   主演: 宋康昊 Kang-ho Song / 金相庆 Sang-kyun/2003 / 韩国 / 犯罪 剧情 悬疑 惊悚</t>
-  </si>
-  <si>
     <t>记忆碎片 / Memento</t>
   </si>
   <si>
@@ -1255,6 +1255,24 @@
     <t>导演: 李安   主演: 赵文瑄 / 归亚蕾 / 金素梅1993 / 台湾 美国 / 剧情 喜剧 爱情 同性 家庭</t>
   </si>
   <si>
+    <t>小森林 夏秋篇 / リトル・フォレスト 夏・秋</t>
+  </si>
+  <si>
+    <t> / 小森食光 / 夏秋篇(台) </t>
+  </si>
+  <si>
+    <t>导演: 森淳一 Junichi Mori   主演: 桥本爱 Ai Hashimoto / 三浦贵大 Takahir/2014 / 日本 / 剧情</t>
+  </si>
+  <si>
+    <t>喜剧之王 / 喜劇之王</t>
+  </si>
+  <si>
+    <t> / King of Comedy</t>
+  </si>
+  <si>
+    <t>导演: 周星驰 Stephen Chow / 李力持 Lik-Chi Lee   主演: 周星驰 Stephen Ch/1999 / 香港 / 喜剧 剧情 爱情</t>
+  </si>
+  <si>
     <t>穿越时空的少女 / 時をかける少女</t>
   </si>
   <si>
@@ -1282,15 +1300,6 @@
     <t>导演: 丹尼·博伊尔 Danny Boyle   主演: 伊万·麦克格雷格 Ewan McGregor / /1996 / 英国 / 犯罪 剧情</t>
   </si>
   <si>
-    <t>小森林 夏秋篇 / リトル・フォレスト 夏・秋</t>
-  </si>
-  <si>
-    <t> / 小森食光 / 夏秋篇(台) </t>
-  </si>
-  <si>
-    <t>导演: 森淳一 Junichi Mori   主演: 桥本爱 Ai Hashimoto / 三浦贵大 Takahir/2014 / 日本 / 剧情</t>
-  </si>
-  <si>
     <t>恋恋笔记本 / The Notebook</t>
   </si>
   <si>
@@ -1300,15 +1309,6 @@
     <t>导演: 尼克·卡索维茨 Nick Cassavetes   主演: 瑞恩·高斯林 Ryan Gosling //2004 / 美国 / 剧情 爱情</t>
   </si>
   <si>
-    <t>喜剧之王 / 喜劇之王</t>
-  </si>
-  <si>
-    <t> / King of Comedy</t>
-  </si>
-  <si>
-    <t>导演: 周星驰 Stephen Chow / 李力持 Lik-Chi Lee   主演: 周星驰 Stephen Ch/1999 / 香港 / 喜剧 剧情 爱情</t>
-  </si>
-  <si>
     <t>英雄本色</t>
   </si>
   <si>
@@ -1399,6 +1399,24 @@
     <t>导演: 杰茜·尼尔森 Jessie Nelson   主演: Sean Penn / Dakota Fanning / Mi/2001 / 美国 / 剧情 家庭</t>
   </si>
   <si>
+    <t>7号房的礼物 / 7번방의 선물</t>
+  </si>
+  <si>
+    <t> / 戆爸的礼物(港)  /  7号囚房的礼物</t>
+  </si>
+  <si>
+    <t>导演: 李焕庆 Hwan-kyeong Lee   主演: 柳承龙 Seung-yong Ryoo / 朴信惠 Shi/2013 / 韩国 / 剧情 喜剧 家庭</t>
+  </si>
+  <si>
+    <t>哈利·波特与死亡圣器(下) / Harry Potter and the Deathly Hallows: Part 2</t>
+  </si>
+  <si>
+    <t> / 哈利波特7：死神的圣物2(港 / 台) </t>
+  </si>
+  <si>
+    <t>导演: 大卫·叶茨 David Yates   主演: 丹尼尔·雷德克里夫 Daniel Radcliffe/2011 / 美国 英国 / 剧情 悬疑 奇幻 冒险</t>
+  </si>
+  <si>
     <t>浪潮 / Die Welle</t>
   </si>
   <si>
@@ -1406,24 +1424,6 @@
   </si>
   <si>
     <t>导演: 丹尼斯·甘塞尔 Dennis Gansel   主演: 尤尔根·沃格尔 Jürgen Vogel /2008 / 德国 / 剧情 惊悚</t>
-  </si>
-  <si>
-    <t>哈利·波特与死亡圣器(下) / Harry Potter and the Deathly Hallows: Part 2</t>
-  </si>
-  <si>
-    <t> / 哈利波特7：死神的圣物2(港 / 台) </t>
-  </si>
-  <si>
-    <t>导演: 大卫·叶茨 David Yates   主演: 丹尼尔·雷德克里夫 Daniel Radcliffe/2011 / 美国 英国 / 剧情 悬疑 奇幻 冒险</t>
-  </si>
-  <si>
-    <t>7号房的礼物 / 7번방의 선물</t>
-  </si>
-  <si>
-    <t> / 戆爸的礼物(港)  /  7号囚房的礼物</t>
-  </si>
-  <si>
-    <t>导演: 李焕庆 Hwan-kyeong Lee   主演: 柳承龙 Seung-yong Ryoo / 朴信惠 Shi/2013 / 韩国 / 剧情 喜剧 家庭</t>
   </si>
   <si>
     <t>花样年华 / 花樣年華</t>
@@ -1518,6 +1518,15 @@
     <t>导演: 黑泽明 Akira Kurosawa   主演: 三船敏郎 Toshirô Mifune / 千秋实 /1950 / 日本 / 犯罪 剧情 悬疑</t>
   </si>
   <si>
+    <t>心迷宫</t>
+  </si>
+  <si>
+    <t> / 殡棺  /  The Coffin in the Mountain</t>
+  </si>
+  <si>
+    <t>导演: 忻钰坤 Yukun Xin   主演: 霍卫民 Weimin Huo / 王笑天 Xiaotian Wang /2014 / 中国大陆 / 剧情 犯罪 悬疑</t>
+  </si>
+  <si>
     <t>时空恋旅人 / About Time</t>
   </si>
   <si>
@@ -1527,15 +1536,6 @@
     <t>导演: 理查德·柯蒂斯 Richard Curtis   主演: 多姆纳尔·格利森 Domhnall Gl/2013 / 英国 / 剧情 爱情 奇幻</t>
   </si>
   <si>
-    <t>心迷宫</t>
-  </si>
-  <si>
-    <t> / 殡棺  /  The Coffin in the Mountain</t>
-  </si>
-  <si>
-    <t>导演: 忻钰坤 Yukun Xin   主演: 霍卫民 Weimin Huo / 王笑天 Xiaotian Wang /2014 / 中国大陆 / 剧情 犯罪 悬疑</t>
-  </si>
-  <si>
     <t>唐伯虎点秋香 / 唐伯虎點秋香</t>
   </si>
   <si>
@@ -1545,6 +1545,15 @@
     <t>导演: 李力持 Lik-Chi Lee   主演: 周星驰 Stephen Chow / 巩俐 Li Gong / 陈/1993 / 香港 / 喜剧 爱情 古装</t>
   </si>
   <si>
+    <t>超能陆战队 / Big Hero 6</t>
+  </si>
+  <si>
+    <t> / 大英雄联盟(港)  /  大英雄天团(台)</t>
+  </si>
+  <si>
+    <t>导演: 唐·霍尔 Don Hall / 克里斯·威廉姆斯 Chris Williams   主演: 斯科特/2014 / 美国 / 喜剧 动作 科幻 动画 冒险</t>
+  </si>
+  <si>
     <t>战争之王 / Lord of War</t>
   </si>
   <si>
@@ -1563,6 +1572,15 @@
     <t>导演: 达伦·阿伦诺夫斯基 Darren Aronofsky   主演: 艾伦·伯斯汀 Ellen Bur/2000 / 美国 / 剧情</t>
   </si>
   <si>
+    <t>可可西里</t>
+  </si>
+  <si>
+    <t> / Kekexili: Mountain Patrol</t>
+  </si>
+  <si>
+    <t>导演: 陆川 Chuan Lu   主演: 多布杰 Duobujie / 张磊 Lei Zhang / 亓亮 Qi L/2004 / 中国大陆 香港 / 剧情 犯罪</t>
+  </si>
+  <si>
     <t>碧海蓝天 / Le grand bleu</t>
   </si>
   <si>
@@ -1572,22 +1590,31 @@
     <t>导演: Luc Besson   主演: Jean-Marc Barr / Jean Reno / Rosanna Arquette1988 / 法国 美国 意大利 / 剧情 爱情</t>
   </si>
   <si>
-    <t>超能陆战队 / Big Hero 6</t>
-  </si>
-  <si>
-    <t> / 大英雄联盟(港)  /  大英雄天团(台)</t>
-  </si>
-  <si>
-    <t>导演: 唐·霍尔 Don Hall / 克里斯·威廉姆斯 Chris Williams   主演: 斯科特/2014 / 美国 / 喜剧 动作 科幻 动画 冒险</t>
-  </si>
-  <si>
-    <t>可可西里</t>
-  </si>
-  <si>
-    <t> / Kekexili: Mountain Patrol</t>
-  </si>
-  <si>
-    <t>导演: 陆川 Chuan Lu   主演: 多布杰 Duobujie / 张磊 Lei Zhang / 亓亮 Qi L/2004 / 中国大陆 香港 / 剧情 犯罪</t>
+    <t>小森林 冬春篇 / リトル・フォレスト 冬・春</t>
+  </si>
+  <si>
+    <t> / 小森食光 / 冬春篇(台) </t>
+  </si>
+  <si>
+    <t>导演: 森淳一 Junichi Mori   主演: 桥本爱 Ai Hashimoto / 三浦贵大 Takahir/2015 / 日本 / 剧情</t>
+  </si>
+  <si>
+    <t>地球上的星星 / Taare Zameen Par</t>
+  </si>
+  <si>
+    <t> / 心中的小星星(台)  /  每一个孩子都是特别的</t>
+  </si>
+  <si>
+    <t>导演: 阿米尔·汗 Aamir Khan   主演: 达席尔·萨法瑞 Darsheel Safary / 阿/2007 / 印度 / 剧情 儿童 家庭</t>
+  </si>
+  <si>
+    <t>蝙蝠侠：黑暗骑士崛起 / The Dark Knight Rises</t>
+  </si>
+  <si>
+    <t> / 蝙蝠侠前传3：黑暗骑士崛起  /  黑暗骑士：黎明升起(台)</t>
+  </si>
+  <si>
+    <t>导演: 克里斯托弗·诺兰 Christopher Nolan   主演: 克里斯蒂安·贝尔 Christ/2012 / 美国 英国 / 剧情 动作 科幻 犯罪 惊悚</t>
   </si>
   <si>
     <t>秒速5厘米 / 秒速5センチメートル</t>
@@ -1599,33 +1626,6 @@
     <t>导演: 新海诚 Makoto Shinkai   主演: 水桥研二 Kenji Mizuhashi / 近藤好美 /2007 / 日本 / 动画 剧情 爱情</t>
   </si>
   <si>
-    <t>地球上的星星 / Taare Zameen Par</t>
-  </si>
-  <si>
-    <t> / 心中的小星星(台)  /  每一个孩子都是特别的</t>
-  </si>
-  <si>
-    <t>导演: 阿米尔·汗 Aamir Khan   主演: 达席尔·萨法瑞 Darsheel Safary / 阿/2007 / 印度 / 剧情 儿童 家庭</t>
-  </si>
-  <si>
-    <t>小森林 冬春篇 / リトル・フォレスト 冬・春</t>
-  </si>
-  <si>
-    <t> / 小森食光 / 冬春篇(台) </t>
-  </si>
-  <si>
-    <t>导演: 森淳一 Junichi Mori   主演: 桥本爱 Ai Hashimoto / 三浦贵大 Takahir/2015 / 日本 / 剧情</t>
-  </si>
-  <si>
-    <t>蝙蝠侠：黑暗骑士崛起 / The Dark Knight Rises</t>
-  </si>
-  <si>
-    <t> / 蝙蝠侠前传3：黑暗骑士崛起  /  黑暗骑士：黎明升起(台)</t>
-  </si>
-  <si>
-    <t>导演: 克里斯托弗·诺兰 Christopher Nolan   主演: 克里斯蒂安·贝尔 Christ/2012 / 美国 英国 / 剧情 动作 科幻 犯罪 惊悚</t>
-  </si>
-  <si>
     <t>海盗电台 / The Boat That Rocked</t>
   </si>
   <si>
@@ -1653,6 +1653,15 @@
     <t>导演: 道格·里曼 Doug Liman   主演: 马特·达蒙 Matt Damon / 弗兰卡·波坦/2002 / 美国 德国 捷克 / 动作 悬疑 惊悚</t>
   </si>
   <si>
+    <t>恐怖游轮 / Triangle</t>
+  </si>
+  <si>
+    <t> / 汪洋血迷宮(台)  /  轮回三角</t>
+  </si>
+  <si>
+    <t>导演: 克里斯托弗·史密斯 Christopher Smith   主演: 梅利莎·乔治 Melissa /2009 / 英国 澳大利亚 / 剧情 悬疑 惊悚</t>
+  </si>
+  <si>
     <t>阿飞正传 / 阿飛正傳</t>
   </si>
   <si>
@@ -1662,15 +1671,6 @@
     <t>导演: 王家卫 Kar Wai Wong   主演: 张国荣 Leslie Cheung / 张曼玉 Maggie C/1990 / 香港 / 犯罪 剧情 爱情</t>
   </si>
   <si>
-    <t>恐怖游轮 / Triangle</t>
-  </si>
-  <si>
-    <t> / 汪洋血迷宮(台)  /  轮回三角</t>
-  </si>
-  <si>
-    <t>导演: 克里斯托弗·史密斯 Christopher Smith   主演: 梅利莎·乔治 Melissa /2009 / 英国 澳大利亚 / 剧情 悬疑 惊悚</t>
-  </si>
-  <si>
     <t>未麻的部屋 / Perfect Blue</t>
   </si>
   <si>
@@ -1698,6 +1698,15 @@
     <t>导演: 让-马克·瓦雷 Jean-Marc Vallée   主演: 马修·麦康纳 Matthew McCon/2013 / 美国 / 剧情 传记 同性</t>
   </si>
   <si>
+    <t>牯岭街少年杀人事件 / 牯嶺街少年殺人事件</t>
+  </si>
+  <si>
+    <t> / A Brighter Summer Day</t>
+  </si>
+  <si>
+    <t>导演: 杨德昌 Edward Yang   主演: 张震 Chen Chang / 杨静怡 Lisa Yang / 张/1991 / 台湾 / 剧情 犯罪</t>
+  </si>
+  <si>
     <t>惊魂记 / Psycho</t>
   </si>
   <si>
@@ -1707,15 +1716,6 @@
     <t>导演: Alfred Hitchcock   主演: Janet Leigh / Anthony Perkins / Vera Miles1960 / 美国 / 悬疑 恐怖</t>
   </si>
   <si>
-    <t>牯岭街少年杀人事件 / 牯嶺街少年殺人事件</t>
-  </si>
-  <si>
-    <t> / A Brighter Summer Day</t>
-  </si>
-  <si>
-    <t>导演: 杨德昌 Edward Yang   主演: 张震 Chen Chang / 杨静怡 Lisa Yang / 张/1991 / 台湾 / 剧情 犯罪</t>
-  </si>
-  <si>
     <t>魔女宅急便 / 魔女の宅急便</t>
   </si>
   <si>
@@ -1725,6 +1725,24 @@
     <t>导演: 宫崎骏 Hayao Miyazaki   主演: 高山南 / 佐久间玲 / 山口胜平1989 / 日本 / 动画 奇幻 冒险</t>
   </si>
   <si>
+    <t>再次出发之纽约遇见你 / Begin Again</t>
+  </si>
+  <si>
+    <t> / 再次出发  /  歌曲改变人生</t>
+  </si>
+  <si>
+    <t>导演: 约翰·卡尼 John Carney   主演: 凯拉·奈特莉 Keira Knightley / 马克/2013 / 美国 / 喜剧 爱情 音乐</t>
+  </si>
+  <si>
+    <t>绿里奇迹 / The Green Mile</t>
+  </si>
+  <si>
+    <t> / 绿色奇迹(台)  /  绿色英里</t>
+  </si>
+  <si>
+    <t>导演: Frank Darabont   主演: 汤姆·汉克斯 Tom Hanks / 大卫·摩斯 David M/1999 / 美国 / 犯罪 剧情 奇幻 悬疑</t>
+  </si>
+  <si>
     <t>迁徙的鸟 / Le peuple migrateur</t>
   </si>
   <si>
@@ -1734,24 +1752,6 @@
     <t>导演: 雅克·贝汉 Jacques Perrin / 雅克·克鲁奥德 Jacques Cluzaud   主演:/2001 / 法国 德国 意大利 西班牙 瑞士 / 纪录片</t>
   </si>
   <si>
-    <t>绿里奇迹 / The Green Mile</t>
-  </si>
-  <si>
-    <t> / 绿色奇迹(台)  /  绿色英里</t>
-  </si>
-  <si>
-    <t>导演: Frank Darabont   主演: 汤姆·汉克斯 Tom Hanks / 大卫·摩斯 David M/1999 / 美国 / 犯罪 剧情 奇幻 悬疑</t>
-  </si>
-  <si>
-    <t>再次出发之纽约遇见你 / Begin Again</t>
-  </si>
-  <si>
-    <t> / 再次出发  /  歌曲改变人生</t>
-  </si>
-  <si>
-    <t>导演: 约翰·卡尼 John Carney   主演: 凯拉·奈特莉 Keira Knightley / 马克/2013 / 美国 / 喜剧 爱情 音乐</t>
-  </si>
-  <si>
     <t>勇闯夺命岛 / The Rock</t>
   </si>
   <si>
@@ -1761,6 +1761,15 @@
     <t>导演: 迈克尔·贝 Michael Bay   主演: 肖恩·康纳利 Sean Connery / 尼古拉/1996 / 美国 / 动作 冒险</t>
   </si>
   <si>
+    <t>海边的曼彻斯特 / Manchester by the Sea</t>
+  </si>
+  <si>
+    <t> / 情系海边之城(港)</t>
+  </si>
+  <si>
+    <t>导演: 肯尼斯·罗纳根 Kenneth Lonergan   主演: 卡西·阿弗莱克 Casey Affle/2016 / 美国 / 剧情 家庭</t>
+  </si>
+  <si>
     <t>荒野生存 / Into the Wild</t>
   </si>
   <si>
@@ -1824,6 +1833,15 @@
     <t>导演: 詹姆斯·卡梅隆 James Cameron   主演: 阿诺·施瓦辛格 Arnold Schwarz/1991 / 美国 法国 / 动作 科幻</t>
   </si>
   <si>
+    <t>青蛇</t>
+  </si>
+  <si>
+    <t> / Green Snake</t>
+  </si>
+  <si>
+    <t>导演: 徐克 Hark Tsui   主演: 张曼玉 Maggie Cheung / 王祖贤 Joey Wang / /1993 / 香港 / 剧情 奇幻 古装</t>
+  </si>
+  <si>
     <t>这个男人来自地球 / The Man from Earth</t>
   </si>
   <si>
@@ -1833,13 +1851,13 @@
     <t>导演: 理查德·沙因克曼 Richard Schenkman   主演: 大卫·李·史密斯 David /2007 / 美国 / 剧情 科幻</t>
   </si>
   <si>
-    <t>青蛇</t>
-  </si>
-  <si>
-    <t> / Green Snake</t>
-  </si>
-  <si>
-    <t>导演: 徐克 Hark Tsui   主演: 张曼玉 Maggie Cheung / 王祖贤 Joey Wang / /1993 / 香港 / 剧情 奇幻 古装</t>
+    <t>忠犬八公物语 / ハチ公物語</t>
+  </si>
+  <si>
+    <t> / 八千公物语  /  阿八的故事</t>
+  </si>
+  <si>
+    <t>导演: Seijirô Kôyama   主演: 山本圭 Kei Yamamoto / 井川比佐志 Hisa/1987 / 日本 / 剧情</t>
   </si>
   <si>
     <t>变脸 / Face/Off</t>
@@ -1851,15 +1869,6 @@
     <t>导演: 吴宇森 John Woo   主演: 约翰·特拉沃尔塔 John Travolta / 尼古拉斯/1997 / 美国 / 动作 科幻 犯罪</t>
   </si>
   <si>
-    <t>忠犬八公物语 / ハチ公物語</t>
-  </si>
-  <si>
-    <t> / 八千公物语  /  阿八的故事</t>
-  </si>
-  <si>
-    <t>导演: Seijirô Kôyama   主演: 山本圭 Kei Yamamoto / 井川比佐志 Hisa/1987 / 日本 / 剧情</t>
-  </si>
-  <si>
     <t>英国病人 / The English Patient</t>
   </si>
   <si>
@@ -1905,6 +1914,15 @@
     <t>导演: 李惠民 Raymond Lee   主演: 张曼玉 Maggie Cheung / 林青霞 Brigitte /1992 / 香港 中国大陆 / 剧情 动作 武侠 古装</t>
   </si>
   <si>
+    <t>黄金三镖客 / Il buono, il brutto, il cattivo.</t>
+  </si>
+  <si>
+    <t> / 好·坏·丑  /  独行侠决斗地狱门(港)</t>
+  </si>
+  <si>
+    <t>导演: Sergio Leone   主演: Clint Eastwood / Eli Wallach / Lee Van Cleef1966 / 意大利 西班牙 西德 / 冒险 西部</t>
+  </si>
+  <si>
     <t>发条橙 / A Clockwork Orange</t>
   </si>
   <si>
@@ -1914,6 +1932,15 @@
     <t>导演: Stanley Kubrick   主演: Malcolm McDowell / Patrick Magee / Michael/1971 / 英国 美国 / 犯罪 剧情 科幻</t>
   </si>
   <si>
+    <t>黑客帝国3：矩阵革命 / The Matrix Revolutions</t>
+  </si>
+  <si>
+    <t> / 骇客任务完结篇：最后战役  /  廿二世纪杀人网络3：惊变世纪</t>
+  </si>
+  <si>
+    <t>导演: Andy Wachowski / Larry Wachowski   主演: Keanu Reeves / Laurence F/2003 / 美国 澳大利亚 / 动作 科幻</t>
+  </si>
+  <si>
     <t>叫我第一名 / Front of the Class</t>
   </si>
   <si>
@@ -1923,24 +1950,6 @@
     <t>导演: 彼得·维纳 Peter Werner   主演: 詹姆斯·沃克 James Wolk / 特里特·/2008 / 美国 / 剧情 传记</t>
   </si>
   <si>
-    <t>黄金三镖客 / Il buono, il brutto, il cattivo.</t>
-  </si>
-  <si>
-    <t> / 好·坏·丑  /  独行侠决斗地狱门(港)</t>
-  </si>
-  <si>
-    <t>导演: Sergio Leone   主演: Clint Eastwood / Eli Wallach / Lee Van Cleef1966 / 意大利 西班牙 西德 / 冒险 西部</t>
-  </si>
-  <si>
-    <t>黑客帝国3：矩阵革命 / The Matrix Revolutions</t>
-  </si>
-  <si>
-    <t> / 骇客任务完结篇：最后战役  /  廿二世纪杀人网络3：惊变世纪</t>
-  </si>
-  <si>
-    <t>导演: Andy Wachowski / Larry Wachowski   主演: Keanu Reeves / Laurence F/2003 / 美国 澳大利亚 / 动作 科幻</t>
-  </si>
-  <si>
     <t>美国丽人 / American Beauty</t>
   </si>
   <si>
@@ -1950,6 +1959,15 @@
     <t>导演: 萨姆·门德斯 Sam Mendes   主演: 凯文·史佩西 Kevin Spacey / 安妮特/1999 / 美国 / 剧情 家庭</t>
   </si>
   <si>
+    <t>城市之光 / City Lights</t>
+  </si>
+  <si>
+    <t> / City Lights: A Comedy Romance in Pantomime  /  Lichter der Großstadt</t>
+  </si>
+  <si>
+    <t>导演: Charles Chaplin   主演: 查理·卓别林 Charles Chaplin / 弗吉尼亚·/1931 / 美国 / 喜剧 剧情 爱情</t>
+  </si>
+  <si>
     <t>穆赫兰道 / Mulholland Dr.</t>
   </si>
   <si>
@@ -1957,15 +1975,6 @@
   </si>
   <si>
     <t>导演: 大卫·林奇 David Lynch   主演: 娜奥米·沃茨 Naomi Watts / 劳拉·哈/2001 / 法国 美国 / 剧情 悬疑 惊悚</t>
-  </si>
-  <si>
-    <t>城市之光 / City Lights</t>
-  </si>
-  <si>
-    <t> / City Lights: A Comedy Romance in Pantomime  /  Lichter der Großstadt</t>
-  </si>
-  <si>
-    <t>导演: Charles Chaplin   主演: 查理·卓别林 Charles Chaplin / 弗吉尼亚·/1931 / 美国 / 喜剧 剧情 爱情</t>
   </si>
   <si>
     <t>非常嫌疑犯 / The Usual Suspects</t>
@@ -2070,31 +2079,43 @@
     <t>导演: 莫腾·泰杜姆 Morten Tyldum   主演: 本尼迪克特·康伯巴奇 Benedict C/2014 / 英国 美国 / 剧情 传记 战争 同性</t>
   </si>
   <si>
+    <t>无敌破坏王 / Wreck-It Ralph</t>
+  </si>
+  <si>
+    <t> / 破坏王拉尔夫  /  破坏王大冒险</t>
+  </si>
+  <si>
+    <t>导演: 瑞奇·莫尔 Rich Moore   主演: 简·林奇 Jane Lynch / 约翰·C·赖利 /2012 / 美国 / 喜剧 动画 冒险</t>
+  </si>
+  <si>
+    <t>大卫·戈尔的一生 / The Life of David Gale</t>
+  </si>
+  <si>
+    <t> / 铁案悬谜  /  命悬一线</t>
+  </si>
+  <si>
+    <t>导演: Alan Parker   主演: 凯文·史派西 Kevin Spacey / 凯特·温丝莱特 Kat/2003 / 美国 德国 英国 / 剧情 犯罪 悬疑</t>
+  </si>
+  <si>
     <t>曾经 / Once</t>
   </si>
   <si>
     <t> / 一奏倾情(港)  /  曾经。爱是唯一(台)</t>
   </si>
   <si>
-    <t>导演: 约翰·卡尼 John Carney   主演: 格伦·汉塞德 Glen Hansard / 玛可塔/2006 / 爱尔兰 / 剧情 音乐 爱情</t>
-  </si>
-  <si>
-    <t>无敌破坏王 / Wreck-It Ralph</t>
-  </si>
-  <si>
-    <t> / 破坏王拉尔夫  /  破坏王大冒险</t>
-  </si>
-  <si>
-    <t>导演: 瑞奇·莫尔 Rich Moore   主演: 简·林奇 Jane Lynch / 约翰·C·赖利 /2012 / 美国 / 喜剧 动画 冒险</t>
-  </si>
-  <si>
-    <t>大卫·戈尔的一生 / The Life of David Gale</t>
-  </si>
-  <si>
-    <t> / 铁案悬谜  /  命悬一线</t>
-  </si>
-  <si>
-    <t>导演: Alan Parker   主演: 凯文·史派西 Kevin Spacey / 凯特·温丝莱特 Kat/2003 / 美国 德国 英国 / 剧情 犯罪 悬疑</t>
+    <t>导演: 约翰·卡尼 John Carney   主演: 格伦·汉塞德 Glen Hansard / 玛可塔/2007 / 爱尔兰 / 剧情 音乐 爱情</t>
+  </si>
+  <si>
+    <t>血钻 / Blood Diamond</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t> / 血腥钻石  /  滴血钻石</t>
+  </si>
+  <si>
+    <t>导演: Edward Zwick   主演: Leonardo DiCaprio / Jennifer Connelly / Djimo/2006 / 美国 德国 / 剧情 惊悚 冒险</t>
   </si>
   <si>
     <t>麦兜故事 / 麥兜故事</t>
@@ -2106,16 +2127,16 @@
     <t>导演: 袁建滔 Toe Yuen   主演: 李晋纬 / 林海峰 Jan Lamb / 吴君如 Sandra Ng2001 / 香港 / 剧情 喜剧 动画</t>
   </si>
   <si>
-    <t>血钻 / Blood Diamond</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t> / 血腥钻石  /  滴血钻石</t>
-  </si>
-  <si>
-    <t>导演: Edward Zwick   主演: Leonardo DiCaprio / Jennifer Connelly / Djimo/2006 / 美国 德国 / 剧情 惊悚 冒险</t>
+    <t>国王的演讲 / The King&amp;#39 s Speech</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t> / 皇上无话儿(港)  /  王者之声：宣战时刻(台)</t>
+  </si>
+  <si>
+    <t>导演: 汤姆·霍珀 Tom Hooper   主演: 柯林·菲尔斯 Colin Firth / 杰弗里·/2010 / 英国 澳大利亚 美国 / 剧情 传记 历史</t>
   </si>
   <si>
     <t>暖暖内含光 / Eternal Sunshine of the Spotless Mind</t>
@@ -2130,67 +2151,79 @@
     <t>导演: 米歇尔·冈瑞 Michel Gondry   主演: 金·凯瑞 Jim Carrey / 凯特·温/2004 / 美国 / 剧情 爱情 奇幻</t>
   </si>
   <si>
-    <t>国王的演讲 / The King&amp;#39 s Speech</t>
-  </si>
-  <si>
-    <t>8.3</t>
-  </si>
-  <si>
-    <t> / 皇上无话儿(港)  /  王者之声：宣战时刻(台)</t>
-  </si>
-  <si>
-    <t>导演: 汤姆·霍珀 Tom Hooper   主演: 柯林·菲尔斯 Colin Firth / 杰弗里·/2010 / 英国 澳大利亚 美国 / 剧情 传记 历史</t>
+    <t>爱在午夜降临前 / Before Midnight</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t> / 爱在午夜希腊时(台)  /  情约半生(港)</t>
+  </si>
+  <si>
+    <t>导演: 理查德·林克莱特 Richard Linklater   主演: 伊桑·霍克 Ethan Hawke /2013 / 美国 / 剧情 爱情</t>
+  </si>
+  <si>
+    <t>枪火 / 鎗火</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t> / The Mission</t>
+  </si>
+  <si>
+    <t>导演: 杜琪峰 Johnnie To   主演: 吴镇宇 Francis Ng / 任达华 Simon Yam / /1999 / 香港 / 剧情 动作 犯罪</t>
   </si>
   <si>
     <t>蝴蝶 / Le Papillon</t>
   </si>
   <si>
-    <t>8.6</t>
-  </si>
-  <si>
     <t> / The Butterfly</t>
   </si>
   <si>
     <t>导演: 菲利普·穆伊尔 Philippe Muyl   主演: 米歇尔·塞罗 Michel Serrault /2002 / 法国 / 剧情 儿童 喜剧</t>
   </si>
   <si>
-    <t>爱在午夜降临前 / Before Midnight</t>
+    <t>遗愿清单 / The Bucket List</t>
+  </si>
+  <si>
+    <t> / 玩转身前事(港)  /  一路玩到挂(台)</t>
+  </si>
+  <si>
+    <t>导演: 罗伯·莱纳 Rob Reiner   主演: 杰克·尼科尔森 Jack Nicholson / 摩根/2007 / 美国 / 冒险 喜剧 剧情</t>
+  </si>
+  <si>
+    <t>疯狂的石头</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t> / Crazy Stone</t>
+  </si>
+  <si>
+    <t>导演: 宁浩 Hao Ning   主演: 郭涛 Tao Guo / 刘桦 Hua Liu / 连晋 Teddy Lin2006 / 中国大陆 香港 / 喜剧 犯罪</t>
+  </si>
+  <si>
+    <t>巴黎淘气帮 / Le petit Nicolas</t>
+  </si>
+  <si>
+    <t> / 小淘气尼古拉(台)  /  反斗小尼哥(港)</t>
+  </si>
+  <si>
+    <t>导演: Laurent Tirard   主演: 马克西姆·戈达尔 Maxime Godart / 瓦莱丽·勒/2009 / 法国 比利时 / 儿童 喜剧 家庭</t>
+  </si>
+  <si>
+    <t>千钧一发 / Gattaca</t>
   </si>
   <si>
     <t>8.7</t>
   </si>
   <si>
-    <t> / 爱在午夜希腊时(台)  /  情约半生(港)</t>
-  </si>
-  <si>
-    <t>导演: 理查德·林克莱特 Richard Linklater   主演: 伊桑·霍克 Ethan Hawke /2013 / 美国 / 剧情 爱情</t>
-  </si>
-  <si>
-    <t>遗愿清单 / The Bucket List</t>
-  </si>
-  <si>
-    <t> / 玩转身前事(港)  /  一路玩到挂(台)</t>
-  </si>
-  <si>
-    <t>导演: 罗伯·莱纳 Rob Reiner   主演: 杰克·尼科尔森 Jack Nicholson / 摩根/2007 / 美国 / 冒险 喜剧 剧情</t>
-  </si>
-  <si>
-    <t>枪火 / 鎗火</t>
-  </si>
-  <si>
-    <t> / The Mission</t>
-  </si>
-  <si>
-    <t>导演: 杜琪峰 Johnnie To   主演: 吴镇宇 Francis Ng / 任达华 Simon Yam / /1999 / 香港 / 剧情 动作 犯罪</t>
-  </si>
-  <si>
-    <t>巴黎淘气帮 / Le petit Nicolas</t>
-  </si>
-  <si>
-    <t> / 小淘气尼古拉(台)  /  反斗小尼哥(港)</t>
-  </si>
-  <si>
-    <t>导演: Laurent Tirard   主演: 马克西姆·戈达尔 Maxime Godart / 瓦莱丽·勒/2009 / 法国 比利时 / 儿童 喜剧 家庭</t>
+    <t> / 变种异煞  /  自然人</t>
+  </si>
+  <si>
+    <t>导演: 安德鲁·尼科尔 Andrew Niccol   主演: 伊桑·霍克 Ethan Hawke / 乌玛/1997 / 美国 / 剧情 科幻</t>
   </si>
   <si>
     <t>与狼共舞 / Dances with Wolves</t>
@@ -2205,27 +2238,6 @@
     <t>导演: Kevin Costner   主演: Kevin Costner / Mary McDonnell / Graham Greene1990 / 美国 / 冒险 剧情 西部</t>
   </si>
   <si>
-    <t>疯狂的石头</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
-    <t> / Crazy Stone</t>
-  </si>
-  <si>
-    <t>导演: 宁浩 Hao Ning   主演: 郭涛 Tao Guo / 刘桦 Hua Liu / 连晋 Teddy Lin2006 / 中国大陆 香港 / 喜剧 犯罪</t>
-  </si>
-  <si>
-    <t>千钧一发 / Gattaca</t>
-  </si>
-  <si>
-    <t> / 变种异煞  /  自然人</t>
-  </si>
-  <si>
-    <t>导演: 安德鲁·尼科尔 Andrew Niccol   主演: 伊桑·霍克 Ethan Hawke / 乌玛/1997 / 美国 / 剧情 科幻</t>
-  </si>
-  <si>
     <t>荒岛余生 / Cast Away</t>
   </si>
   <si>
@@ -2262,37 +2274,25 @@
     <t>导演: 尼尔·乔丹 Neil Jordan   主演: 布拉德·皮特 Brad Pitt / 汤姆·克鲁/1994 / 美国 / 剧情 奇幻 惊悚</t>
   </si>
   <si>
+    <t>我爱你 / 그대를 사랑합니다</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t> / 爱你  /  Late Blossom</t>
+  </si>
+  <si>
+    <t>导演: 秋昌民 Chang-min Choo   主演: 宋在河 Jae-ho Song / 李顺载 Soon-jae/2011 / 韩国 / 剧情 爱情</t>
+  </si>
+  <si>
     <t>寿司之神 / Jiro Dreams of Sushi</t>
   </si>
   <si>
-    <t>8.8</t>
-  </si>
-  <si>
     <t> / 次郎的寿司梦  /  梦见寿司的次郎</t>
   </si>
   <si>
     <t>导演: 大卫·贾柏 David Gelb   主演: 小野二郎Jiro Ono / 小野祯一 Yoshik/2011 / 美国 / 纪录片</t>
-  </si>
-  <si>
-    <t>我爱你 / 그대를 사랑합니다</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t> / 爱你  /  Late Blossom</t>
-  </si>
-  <si>
-    <t>导演: 秋昌民 Chang-min Choo   主演: 宋在河 Jae-ho Song / 李顺载 Soon-jae/2011 / 韩国 / 剧情 爱情</t>
-  </si>
-  <si>
-    <t>中央车站 / Central do Brasil</t>
-  </si>
-  <si>
-    <t> / 千年等一天  /  Central Station</t>
-  </si>
-  <si>
-    <t>导演: Walter Salles   主演: Fernanda Montenegro / Marília Pêra / Viní/1998 / 巴西 法国 / 剧情</t>
   </si>
   <si>
     <r>
@@ -2315,6 +2315,15 @@
     <t>导演: 楚克‧萨克瑞科 Chukiat Sakveerakul   主演: 维特维斯特·海伦亚沃/2007 / 泰国 / 剧情 爱情 同性 家庭</t>
   </si>
   <si>
+    <t>中央车站 / Central do Brasil</t>
+  </si>
+  <si>
+    <t> / 千年等一天  /  Central Station</t>
+  </si>
+  <si>
+    <t>导演: Walter Salles   主演: Fernanda Montenegro / Marília Pêra / Viní/1998 / 巴西 法国 / 剧情</t>
+  </si>
+  <si>
     <t>廊桥遗梦 / The Bridges of Madison County</t>
   </si>
   <si>
@@ -2324,6 +2333,24 @@
     <t>导演: 克林特·伊斯特伍德 Clint Eastwood   主演: 克林特·伊斯特伍德 Clint/1995 / 美国 / 剧情 爱情</t>
   </si>
   <si>
+    <t>房间 / Room</t>
+  </si>
+  <si>
+    <t> / 不存在的房间(台)  /  抖室(港)</t>
+  </si>
+  <si>
+    <t>导演: 伦尼·阿伯拉罕森 Lenny Abrahamson   主演: 布丽·拉尔森 Brie Larson/2015 / 爱尔兰 加拿大 / 剧情 家庭</t>
+  </si>
+  <si>
+    <t>头脑特工队 / Inside Out</t>
+  </si>
+  <si>
+    <t> / 玩转脑朋友(港)  /  脑筋急转弯(台)</t>
+  </si>
+  <si>
+    <t>导演: 彼特·道格特 Pete Docter / 罗纳尔多·德尔·卡门 Ronaldo Del Carmen  &amp;nb/2015 / 美国 / 喜剧 动画 冒险</t>
+  </si>
+  <si>
     <t>彗星来的那一夜 / Coherence</t>
   </si>
   <si>
@@ -2340,33 +2367,6 @@
   </si>
   <si>
     <t>导演: 弗兰克·米勒 Frank Miller / 罗伯特·罗德里格兹 Robert Rodriguez   /2005 / 美国 / 动作 犯罪 惊悚</t>
-  </si>
-  <si>
-    <t>头脑特工队 / Inside Out</t>
-  </si>
-  <si>
-    <t> / 玩转脑朋友(港)  /  脑筋急转弯(台)</t>
-  </si>
-  <si>
-    <t>导演: 彼特·道格特 Pete Docter / 罗纳尔多·德尔·卡门 Ronaldo Del Carmen  &amp;nb/2015 / 美国 / 喜剧 动画 冒险 家庭</t>
-  </si>
-  <si>
-    <t>房间 / Room</t>
-  </si>
-  <si>
-    <t> / 不存在的房间(台)  /  抖室(港)</t>
-  </si>
-  <si>
-    <t>导演: 伦尼·阿伯拉罕森 Lenny Abrahamson   主演: 布丽·拉尔森 Brie Larson/2015 / 爱尔兰 加拿大 / 剧情 家庭</t>
-  </si>
-  <si>
-    <t>黑鹰坠落 / Black Hawk Down</t>
-  </si>
-  <si>
-    <t> / 黑鹰降落  /  黑鹰计划</t>
-  </si>
-  <si>
-    <t>导演: 雷德利·斯科特 Ridley Scott   主演: 乔什·哈奈特 Josh Hartnett / /2001 / 美国 / 动作 历史 战争</t>
   </si>
 </sst>
 </file>
@@ -2491,18 +2491,17 @@
   </sheetPr>
   <dimension ref="A1:E251"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67136150234742"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1971830985915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.9953051643192"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67136150234742"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3615023474178"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="105.220657276995"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.67136150234742"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2910798122066"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.67136150234742"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +2815,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>56</v>
@@ -3003,7 +3002,7 @@
         <v>88</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>89</v>
@@ -3037,7 +3036,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>95</v>
@@ -3394,7 +3393,7 @@
         <v>157</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>9.1</v>
+        <v>9.6</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>158</v>
@@ -3411,7 +3410,7 @@
         <v>160</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>9.6</v>
+        <v>9.1</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>161</v>
@@ -3428,7 +3427,7 @@
         <v>163</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>8.7</v>
+        <v>9</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>164</v>
@@ -3445,7 +3444,7 @@
         <v>166</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>9</v>
+        <v>8.7</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>167</v>
@@ -3462,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>170</v>
@@ -3479,7 +3478,7 @@
         <v>172</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>9.1</v>
+        <v>8.9</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>173</v>
@@ -3556,7 +3555,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>214</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>215</v>
@@ -3734,7 +3733,7 @@
         <v>217</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>8.8</v>
+        <v>8.7</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>218</v>
@@ -3751,7 +3750,7 @@
         <v>220</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>8.7</v>
+        <v>9.2</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>221</v>
@@ -3768,7 +3767,7 @@
         <v>223</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>8.9</v>
+        <v>8.7</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>224</v>
@@ -3785,7 +3784,7 @@
         <v>226</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>9.2</v>
+        <v>8.9</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>227</v>
@@ -3853,7 +3852,7 @@
         <v>238</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>8.8</v>
+        <v>8.7</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>239</v>
@@ -3870,7 +3869,7 @@
         <v>241</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>242</v>
@@ -3989,7 +3988,7 @@
         <v>262</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>8.8</v>
+        <v>8.6</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>263</v>
@@ -4023,7 +4022,7 @@
         <v>268</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>8.6</v>
+        <v>8.8</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>269</v>
@@ -4346,7 +4345,7 @@
         <v>325</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>8.8</v>
+        <v>8.9</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>326</v>
@@ -4380,7 +4379,7 @@
         <v>331</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>9</v>
+        <v>8.7</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>332</v>
@@ -4397,7 +4396,7 @@
         <v>334</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>335</v>
@@ -4414,7 +4413,7 @@
         <v>337</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>338</v>
@@ -4567,7 +4566,7 @@
         <v>364</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>8.8</v>
+        <v>8.7</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>365</v>
@@ -4584,7 +4583,7 @@
         <v>367</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>368</v>
@@ -4635,7 +4634,7 @@
         <v>376</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>8.5</v>
+        <v>8.8</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>377</v>
@@ -4652,7 +4651,7 @@
         <v>379</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>8.8</v>
+        <v>8.5</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>380</v>
@@ -4669,7 +4668,7 @@
         <v>382</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>8.9</v>
+        <v>8.6</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>383</v>
@@ -4703,7 +4702,7 @@
         <v>388</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>389</v>
@@ -4822,7 +4821,7 @@
         <v>409</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>410</v>
@@ -4839,7 +4838,7 @@
         <v>412</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>8.8</v>
+        <v>8.5</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>413</v>
@@ -4856,7 +4855,7 @@
         <v>415</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>416</v>
@@ -4873,7 +4872,7 @@
         <v>418</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>8.9</v>
+        <v>8.8</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>419</v>
@@ -5349,7 +5348,7 @@
         <v>502</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="D168" s="0" t="s">
         <v>503</v>
@@ -5366,7 +5365,7 @@
         <v>505</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>8.7</v>
+        <v>8.5</v>
       </c>
       <c r="D169" s="0" t="s">
         <v>506</v>
@@ -5417,7 +5416,7 @@
         <v>514</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>8.6</v>
+        <v>8.7</v>
       </c>
       <c r="D172" s="0" t="s">
         <v>515</v>
@@ -5434,7 +5433,7 @@
         <v>517</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>8.3</v>
+        <v>8.9</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>518</v>
@@ -5468,7 +5467,7 @@
         <v>523</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>8.9</v>
+        <v>8.5</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>524</v>
@@ -5485,7 +5484,7 @@
         <v>526</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>8.5</v>
+        <v>8.3</v>
       </c>
       <c r="D176" s="0" t="s">
         <v>527</v>
@@ -5553,7 +5552,7 @@
         <v>538</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>8.5</v>
+        <v>8.3</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>539</v>
@@ -5570,7 +5569,7 @@
         <v>541</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>8.3</v>
+        <v>8.5</v>
       </c>
       <c r="D181" s="0" t="s">
         <v>542</v>
@@ -5638,7 +5637,7 @@
         <v>553</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>8.8</v>
+        <v>8.7</v>
       </c>
       <c r="D185" s="0" t="s">
         <v>554</v>
@@ -5655,7 +5654,7 @@
         <v>556</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>557</v>
@@ -5689,7 +5688,7 @@
         <v>562</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>9.1</v>
+        <v>8.5</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>563</v>
@@ -5723,7 +5722,7 @@
         <v>568</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>8.5</v>
+        <v>9.1</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>569</v>
@@ -5774,7 +5773,7 @@
         <v>577</v>
       </c>
       <c r="C193" s="0" t="n">
-        <v>9.2</v>
+        <v>8.6</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>578</v>
@@ -5791,7 +5790,7 @@
         <v>580</v>
       </c>
       <c r="C194" s="0" t="n">
-        <v>8.5</v>
+        <v>9.2</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>581</v>
@@ -5808,7 +5807,7 @@
         <v>583</v>
       </c>
       <c r="C195" s="0" t="n">
-        <v>8.7</v>
+        <v>8.5</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>584</v>
@@ -5825,7 +5824,7 @@
         <v>586</v>
       </c>
       <c r="C196" s="0" t="n">
-        <v>8.6</v>
+        <v>8.7</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>587</v>
@@ -5859,7 +5858,7 @@
         <v>592</v>
       </c>
       <c r="C198" s="0" t="n">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>593</v>
@@ -5910,7 +5909,7 @@
         <v>601</v>
       </c>
       <c r="C201" s="0" t="n">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="D201" s="0" t="s">
         <v>602</v>
@@ -5961,7 +5960,7 @@
         <v>610</v>
       </c>
       <c r="C204" s="0" t="n">
-        <v>8.8</v>
+        <v>8.4</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>611</v>
@@ -5978,7 +5977,7 @@
         <v>613</v>
       </c>
       <c r="C205" s="0" t="n">
-        <v>8.5</v>
+        <v>8.8</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>614</v>
@@ -5995,7 +5994,7 @@
         <v>616</v>
       </c>
       <c r="C206" s="0" t="n">
-        <v>8.3</v>
+        <v>8.5</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>617</v>
@@ -6012,7 +6011,7 @@
         <v>619</v>
       </c>
       <c r="C207" s="0" t="n">
-        <v>8.4</v>
+        <v>8.3</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>620</v>
@@ -6046,7 +6045,7 @@
         <v>625</v>
       </c>
       <c r="C209" s="0" t="n">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>626</v>
@@ -6063,7 +6062,7 @@
         <v>628</v>
       </c>
       <c r="C210" s="0" t="n">
-        <v>9.1</v>
+        <v>8.4</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>629</v>
@@ -6097,7 +6096,7 @@
         <v>634</v>
       </c>
       <c r="C212" s="0" t="n">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="D212" s="0" t="s">
         <v>635</v>
@@ -6114,7 +6113,7 @@
         <v>637</v>
       </c>
       <c r="C213" s="0" t="n">
-        <v>8.3</v>
+        <v>8.4</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>638</v>
@@ -6148,7 +6147,7 @@
         <v>643</v>
       </c>
       <c r="C215" s="0" t="n">
-        <v>8.6</v>
+        <v>8.3</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>644</v>
@@ -6165,7 +6164,7 @@
         <v>646</v>
       </c>
       <c r="C216" s="0" t="n">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="D216" s="0" t="s">
         <v>647</v>
@@ -6182,7 +6181,7 @@
         <v>649</v>
       </c>
       <c r="C217" s="0" t="n">
-        <v>8.6</v>
+        <v>8.4</v>
       </c>
       <c r="D217" s="0" t="s">
         <v>650</v>
@@ -6199,7 +6198,7 @@
         <v>652</v>
       </c>
       <c r="C218" s="0" t="n">
-        <v>8.2</v>
+        <v>8.6</v>
       </c>
       <c r="D218" s="0" t="s">
         <v>653</v>
@@ -6216,7 +6215,7 @@
         <v>655</v>
       </c>
       <c r="C219" s="0" t="n">
-        <v>8.9</v>
+        <v>8.2</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>656</v>
@@ -6233,7 +6232,7 @@
         <v>658</v>
       </c>
       <c r="C220" s="0" t="n">
-        <v>8.3</v>
+        <v>8.9</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>659</v>
@@ -6250,7 +6249,7 @@
         <v>661</v>
       </c>
       <c r="C221" s="0" t="n">
-        <v>9</v>
+        <v>8.3</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>662</v>
@@ -6267,7 +6266,7 @@
         <v>664</v>
       </c>
       <c r="C222" s="0" t="n">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>665</v>
@@ -6284,7 +6283,7 @@
         <v>667</v>
       </c>
       <c r="C223" s="0" t="n">
-        <v>8.3</v>
+        <v>8.5</v>
       </c>
       <c r="D223" s="0" t="s">
         <v>668</v>
@@ -6335,7 +6334,7 @@
         <v>676</v>
       </c>
       <c r="C226" s="0" t="n">
-        <v>8.5</v>
+        <v>8.3</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>677</v>
@@ -6369,13 +6368,13 @@
         <v>683</v>
       </c>
       <c r="C228" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="D228" s="0" t="s">
         <v>684</v>
       </c>
-      <c r="D228" s="0" t="s">
+      <c r="E228" s="0" t="s">
         <v>685</v>
-      </c>
-      <c r="E228" s="0" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6383,16 +6382,16 @@
         <v>228</v>
       </c>
       <c r="B229" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="C229" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="C229" s="0" t="s">
+      <c r="D229" s="0" t="s">
         <v>688</v>
       </c>
-      <c r="D229" s="0" t="s">
+      <c r="E229" s="0" t="s">
         <v>689</v>
-      </c>
-      <c r="E229" s="0" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6400,16 +6399,16 @@
         <v>229</v>
       </c>
       <c r="B230" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="C230" s="0" t="s">
         <v>691</v>
       </c>
-      <c r="C230" s="0" t="s">
+      <c r="D230" s="0" t="s">
         <v>692</v>
       </c>
-      <c r="D230" s="0" t="s">
+      <c r="E230" s="0" t="s">
         <v>693</v>
-      </c>
-      <c r="E230" s="0" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6417,16 +6416,16 @@
         <v>230</v>
       </c>
       <c r="B231" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="C231" s="0" t="s">
         <v>695</v>
       </c>
-      <c r="C231" s="0" t="s">
+      <c r="D231" s="0" t="s">
         <v>696</v>
       </c>
-      <c r="D231" s="0" t="s">
+      <c r="E231" s="0" t="s">
         <v>697</v>
-      </c>
-      <c r="E231" s="0" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6434,10 +6433,10 @@
         <v>231</v>
       </c>
       <c r="B232" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="C232" s="0" t="s">
         <v>699</v>
-      </c>
-      <c r="C232" s="0" t="s">
-        <v>680</v>
       </c>
       <c r="D232" s="0" t="s">
         <v>700</v>
@@ -6454,7 +6453,7 @@
         <v>702</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="D233" s="0" t="s">
         <v>703</v>
@@ -6471,7 +6470,7 @@
         <v>705</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>692</v>
+        <v>680</v>
       </c>
       <c r="D234" s="0" t="s">
         <v>706</v>
@@ -6505,13 +6504,13 @@
         <v>712</v>
       </c>
       <c r="C236" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="D236" s="0" t="s">
         <v>713</v>
       </c>
-      <c r="D236" s="0" t="s">
+      <c r="E236" s="0" t="s">
         <v>714</v>
-      </c>
-      <c r="E236" s="0" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6519,10 +6518,10 @@
         <v>236</v>
       </c>
       <c r="B237" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="C237" s="0" t="s">
         <v>716</v>
-      </c>
-      <c r="C237" s="0" t="s">
-        <v>696</v>
       </c>
       <c r="D237" s="0" t="s">
         <v>717</v>
@@ -6539,13 +6538,13 @@
         <v>719</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>684</v>
+        <v>720</v>
       </c>
       <c r="D238" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="E238" s="0" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6553,16 +6552,16 @@
         <v>238</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>680</v>
+        <v>691</v>
       </c>
       <c r="D239" s="0" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E239" s="0" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,16 +6569,16 @@
         <v>239</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C240" s="0" t="s">
         <v>680</v>
       </c>
       <c r="D240" s="0" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E240" s="0" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6587,16 +6586,16 @@
         <v>240</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E241" s="0" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6604,10 +6603,10 @@
         <v>241</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>732</v>
+        <v>687</v>
       </c>
       <c r="D242" s="0" t="s">
         <v>733</v>
@@ -6641,7 +6640,7 @@
         <v>739</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D244" s="0" t="s">
         <v>740</v>
@@ -6658,7 +6657,7 @@
         <v>742</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D245" s="0" t="s">
         <v>743</v>
@@ -6675,7 +6674,7 @@
         <v>745</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>680</v>
+        <v>716</v>
       </c>
       <c r="D246" s="0" t="s">
         <v>746</v>
@@ -6692,7 +6691,7 @@
         <v>748</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D247" s="0" t="s">
         <v>749</v>
@@ -6709,7 +6708,7 @@
         <v>751</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>684</v>
+        <v>695</v>
       </c>
       <c r="D248" s="0" t="s">
         <v>752</v>
@@ -6726,7 +6725,7 @@
         <v>754</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>696</v>
+        <v>716</v>
       </c>
       <c r="D249" s="0" t="s">
         <v>755</v>
@@ -6743,7 +6742,7 @@
         <v>757</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>732</v>
+        <v>691</v>
       </c>
       <c r="D250" s="0" t="s">
         <v>758</v>
@@ -6760,7 +6759,7 @@
         <v>760</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>680</v>
+        <v>691</v>
       </c>
       <c r="D251" s="0" t="s">
         <v>761</v>

</xml_diff>